<commit_message>
Added Steady State FEA CFLayup analysis plus some formatting edits
</commit_message>
<xml_diff>
--- a/Analysis/FEA/FEA_Full_Tank_Model_Analysis_Workbook.xlsx
+++ b/Analysis/FEA/FEA_Full_Tank_Model_Analysis_Workbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\khensu\Home01\nab2\Desktop\Git\composite-propellant-tank\Analysis\FEA\Full_Tank_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\khensu\Home01\nab2\Desktop\Git\composite-propellant-tank\Analysis\FEA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3898,15 +3898,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B7:J7"/>
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B13:T13"/>
     <mergeCell ref="K15:U15"/>
     <mergeCell ref="K5:S5"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B7:J7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>

</xml_diff>